<commit_message>
State of last presentation(email) + few changes to tables and introductory texts
</commit_message>
<xml_diff>
--- a/admin/lists/Mailadressen.xlsx
+++ b/admin/lists/Mailadressen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Nachname</t>
   </si>
@@ -26,6 +26,15 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Anneliese</t>
+  </si>
+  <si>
+    <t>annelise@gmx.de</t>
+  </si>
+  <si>
     <t>Blobfisch</t>
   </si>
   <si>
@@ -35,37 +44,46 @@
     <t>Blobfisch@fischteich.de</t>
   </si>
   <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Max@mustermann.de</t>
-  </si>
-  <si>
-    <t>Mia</t>
-  </si>
-  <si>
-    <t>Mia@mustermann.de</t>
-  </si>
-  <si>
-    <t>Röckelein</t>
-  </si>
-  <si>
-    <t>Nina</t>
-  </si>
-  <si>
-    <t>nina-roeckelein@hotmail.de</t>
-  </si>
-  <si>
-    <t>Singer</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Sarah-singer@family.de</t>
+    <t>Caloni</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Caloni@gmx.de</t>
+  </si>
+  <si>
+    <t>Domini</t>
+  </si>
+  <si>
+    <t>Dorothea</t>
+  </si>
+  <si>
+    <t>Domini@gmx.de</t>
+  </si>
+  <si>
+    <t>Emil</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Fabian</t>
+  </si>
+  <si>
+    <t>Fabian@gmx.de</t>
+  </si>
+  <si>
+    <t>Gans</t>
+  </si>
+  <si>
+    <t>Gustav</t>
+  </si>
+  <si>
+    <t>Gans@gmx.de</t>
   </si>
 </sst>
 </file>
@@ -404,7 +422,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,35 +465,57 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>